<commit_message>
Second batch of data updates
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\VoaSL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/20210316_3.2 schema/eps-mex2021-pre_build_20210316/InputData/add-outputs/VoaSL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE9CCC39-2AD7-E04C-9B6E-1F3869E53B8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="975" windowWidth="25830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="14240" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
+    <sheet name="Mexico" sheetId="4" r:id="rId2"/>
+    <sheet name="VoaSL" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,35 +33,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>VoaSL Value of a Statistical Life</t>
   </si>
   <si>
-    <t>Source:</t>
-  </si>
-  <si>
-    <t>U.S. Environmental Protection Agency</t>
-  </si>
-  <si>
-    <t>Frequently Asked Questions on Mortality Risk Valuation</t>
-  </si>
-  <si>
-    <t>We adjust 2006 dollars to 2012 dollars using the following conversion factor:</t>
-  </si>
-  <si>
     <t>See "cpi.xlsx" in the InputData folder for source information.</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>"What value of statistical life does EPA use?"</t>
-  </si>
-  <si>
     <t>Statistical Life</t>
   </si>
   <si>
+    <t>Value (2012$)</t>
+  </si>
+  <si>
     <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
   </si>
   <si>
@@ -75,20 +65,85 @@
     <t>Currency Year Adjustment</t>
   </si>
   <si>
-    <t>2012$/life</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
+    <t>Mexico:</t>
+  </si>
+  <si>
+    <t>INECC - Instituto Nacional de Ecología y Cambio Climático</t>
+  </si>
+  <si>
+    <t>PROAIRE - Megalópolis 2017-2030</t>
+  </si>
+  <si>
+    <t>https://framework-gb.cdn.gob.mx/data/institutos/semarnat/Programa_de_Gesti%C3%B3n_Federal_2017-2030_final.pdf</t>
+  </si>
+  <si>
+    <t>III. IMPACTOS DE LA CONTAMINACIÓN ATMOSFÉRICA, pg.96</t>
+  </si>
+  <si>
+    <t>Central Mexico Megalopolis - Air quality program numbers</t>
+  </si>
+  <si>
+    <t>Value of a statistical Life (VSL)</t>
+  </si>
+  <si>
+    <t>Valores de una Vida Estadística “VVE” seleccionados para el estudio: 1.6 millones de pesos y 13.85 millones de pesos (MXN, 2014), respectivamente. El primero corresponde a un VVE local que resulta del estudio de valoración contingente más reciente que se haya realizado en México, en tanto que el segundo corresponde a un VVE estimado internacionalmente ajustado por ingreso para México y que ha sido usado con anterioridad en diversos análisis de este tipo en el país (INECC, 2016c).</t>
+  </si>
+  <si>
+    <t>MXN, 2014</t>
+  </si>
+  <si>
+    <t>USD, 2012</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VSL1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Local contingency valuation study</t>
+    </r>
+  </si>
+  <si>
+    <t>VSL2 - International estimate, adjusted to Mexico</t>
+  </si>
+  <si>
+    <t>USD, 2014</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>MXN/USD</t>
+  </si>
+  <si>
+    <t>We adjust 2014 dollars to 2012 dollars using the following conversion factor:</t>
+  </si>
+  <si>
+    <t>Currency conversions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +167,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,11 +192,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -145,8 +208,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -484,99 +555,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.97135205460935392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2006</v>
+      </c>
+      <c r="B22">
+        <v>10.901017260273969</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2007</v>
+      </c>
+      <c r="B23">
+        <v>10.926903013698627</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2008</v>
+      </c>
+      <c r="B24">
+        <v>11.138301912568313</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2009</v>
+      </c>
+      <c r="B25">
+        <v>13.509501369863028</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2010</v>
+      </c>
+      <c r="B26">
+        <v>12.636678082191793</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2011</v>
+      </c>
+      <c r="B27">
+        <v>12.427292876712329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2012</v>
+      </c>
+      <c r="B28">
+        <v>13.168531967213106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>2013</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
+      <c r="B29">
+        <v>12.767464383561641</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2014</v>
+      </c>
+      <c r="B30">
+        <v>13.298290410958895</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2015</v>
+      </c>
+      <c r="B31">
+        <v>15.854175890410984</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2016</v>
+      </c>
+      <c r="B32">
+        <v>18.656701092896164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2017</v>
+      </c>
+      <c r="B33">
+        <v>18.929111232876703</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2018</v>
+      </c>
+      <c r="B34">
+        <v>18.822825165562914</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" location="whatvalue" display="https://www.epa.gov/environmental-economics/mortality-risk-valuation - whatvalue" xr:uid="{F4EA8DF9-36E3-4A47-8B4C-6E99399B200A}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -585,36 +780,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1600000</v>
+      </c>
+      <c r="D8" s="7">
+        <f>C8/About!$B$30</f>
+        <v>120316.21738997873</v>
+      </c>
+      <c r="E8" s="6">
+        <f>D8*About!$A$17</f>
+        <v>116869.40496458152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="7">
+        <v>13850000</v>
+      </c>
+      <c r="D9" s="7">
+        <f>C9/About!$B$30</f>
+        <v>1041487.2567820033</v>
+      </c>
+      <c r="E9" s="8">
+        <f>D9*About!$A$17</f>
+        <v>1011650.7867246587</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:F5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <f>7.4*10^6*About!A17</f>
-        <v>8443400</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="9">
+        <f>Mexico!E9</f>
+        <v>1011650.7867246587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>